<commit_message>
slightly better VSWR debug
</commit_message>
<xml_diff>
--- a/measurements/24032020 vswr bridge.xlsx
+++ b/measurements/24032020 vswr bridge.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="37">
   <si>
     <t>Aries VSWR tests</t>
   </si>
@@ -56,12 +56,6 @@
     <t>1:1</t>
   </si>
   <si>
-    <t>Fadc</t>
-  </si>
-  <si>
-    <t>Radc</t>
-  </si>
-  <si>
     <t>dig VSWR</t>
   </si>
   <si>
@@ -75,6 +69,72 @@
   </si>
   <si>
     <t xml:space="preserve">VSWR bridge connected to relays and L/C </t>
+  </si>
+  <si>
+    <t>Vf (ADC)</t>
+  </si>
+  <si>
+    <t>Vr (ADC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSWR bridge connected to relays and L/C, RL1 issue resolved </t>
+  </si>
+  <si>
+    <t>VSWR on LCD display</t>
+  </si>
+  <si>
+    <t>2.4-2.8</t>
+  </si>
+  <si>
+    <t>3.0-3.9</t>
+  </si>
+  <si>
+    <t>There is still a lot of noise on the ADC reasings from the Arduino. Is this because there is RF breakthrough?</t>
+  </si>
+  <si>
+    <t>The huge VSWR errors with high impedance loads have gone. VSWR approximately correct.</t>
+  </si>
+  <si>
+    <t>26/3/2020: VSWR bridge isolated, to "bypass" RF connector. L13 bypassed by wire.</t>
+  </si>
+  <si>
+    <t>1.9MHz</t>
+  </si>
+  <si>
+    <t>typical noise on Fwd ADC measurement +/- 3 samples; on Rev ADC +/-8 samples</t>
+  </si>
+  <si>
+    <t>These appear to be good measurements.</t>
+  </si>
+  <si>
+    <t>28MHz</t>
+  </si>
+  <si>
+    <t>typical noise on Fwd ADC measurement +/- 2 samples; on Rev ADC +/-4 samples</t>
+  </si>
+  <si>
+    <t>The multimeter measurements are useless; Vf exceeds Vr. I suspect there is RF in the multimeter leads.</t>
+  </si>
+  <si>
+    <t>The digital measurements have error but are measuring VSWR, inaccurately</t>
+  </si>
+  <si>
+    <t>25/3/2020: VSWR bridge connected to relays and L/C , RL1 resolved, L13 bypassed by wire</t>
+  </si>
+  <si>
+    <t>26/3/2020: VSWR bridge connected to ATU. L13 bypassed by wire.</t>
+  </si>
+  <si>
+    <t>typical noise on Fwd ADC measurement +/- 7 samples (low Z) +/- 20 sample (high Z)</t>
+  </si>
+  <si>
+    <t>typical noise on Rev ADC measurement +/- 20 samples (low Z) +/- 40 samples (high Z)</t>
+  </si>
+  <si>
+    <t>typical noise on Fwd ADC measurement +/- 6 samples; on Rev ADC +/-40 samples</t>
+  </si>
+  <si>
+    <t>These measurements suggest the bridge is inoperable at 28MHz. Vr &gt;&gt; Vf.</t>
   </si>
 </sst>
 </file>
@@ -82,12 +142,25 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -128,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -138,9 +211,35 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -423,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,20 +540,20 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -473,13 +572,13 @@
         <v>5</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -680,20 +779,20 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+      <c r="C15" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -712,13 +811,13 @@
         <v>5</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -834,96 +933,1581 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="A21" s="7">
         <v>100</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="7">
         <v>0.97199999999999998</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="7">
         <v>0.48499999999999999</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="9">
         <f t="shared" si="2"/>
         <v>2.9917864476386034</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="10">
         <v>1235</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="10">
         <v>620</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="9">
         <f t="shared" si="3"/>
         <v>3.0162601626016259</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="A22" s="7">
         <v>150</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="7">
         <v>1.002</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="7">
         <v>0.73499999999999999</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="9">
         <f t="shared" si="2"/>
         <v>6.5056179775280896</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="10">
         <v>1315</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="10">
         <v>960</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="9">
         <f t="shared" si="3"/>
         <v>6.408450704225352</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+      <c r="A23" s="7">
         <v>200</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="7">
         <v>1.0880000000000001</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="7">
         <v>0.88400000000000001</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="9">
         <f t="shared" si="2"/>
         <v>9.6666666666666625</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="10">
         <v>1366</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="10">
         <v>1105</v>
       </c>
-      <c r="H23" s="5">
+      <c r="H23" s="9">
         <f t="shared" si="3"/>
         <v>9.4674329501915704</v>
       </c>
     </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+    </row>
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="E30" s="5">
+        <f>(C30+D30)/(C30-D30)</f>
+        <v>3.3293413173652699</v>
+      </c>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="18"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>16.7</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0.314</v>
+      </c>
+      <c r="E31" s="5">
+        <f t="shared" ref="E31:E36" si="4">(C31+D31)/(C31-D31)</f>
+        <v>2.4638694638694636</v>
+      </c>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="18"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>25</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="E32" s="5">
+        <f t="shared" si="4"/>
+        <v>1.605042016806723</v>
+      </c>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="18"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>50</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="D33" s="3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="E33" s="5">
+        <f t="shared" si="4"/>
+        <v>1.2204928664072632</v>
+      </c>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="18"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <v>100</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="7">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="D34" s="7">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="E34" s="9">
+        <f t="shared" si="4"/>
+        <v>2.9005964214711732</v>
+      </c>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="20"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>150</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="7">
+        <v>1.052</v>
+      </c>
+      <c r="D35" s="7">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="E35" s="9">
+        <f t="shared" si="4"/>
+        <v>5.3951367781155</v>
+      </c>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="20"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
+        <v>200</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="7">
+        <v>1.095</v>
+      </c>
+      <c r="D36" s="7">
+        <v>0.873</v>
+      </c>
+      <c r="E36" s="9">
+        <f t="shared" si="4"/>
+        <v>8.8648648648648649</v>
+      </c>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="20"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C41" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="25"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I42" s="26"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="3">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="E43" s="5">
+        <f>(C43+D43)/(C43-D43)</f>
+        <v>3.6179401993355489</v>
+      </c>
+      <c r="F43" s="6">
+        <v>893</v>
+      </c>
+      <c r="G43" s="6">
+        <v>504</v>
+      </c>
+      <c r="H43" s="5">
+        <f>(F43+G43)/(F43-G43)</f>
+        <v>3.5912596401028276</v>
+      </c>
+      <c r="I43" s="3">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>16.7</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="3">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="E44" s="5">
+        <f t="shared" ref="E44:E49" si="5">(C44+D44)/(C44-D44)</f>
+        <v>2.7486910994764404</v>
+      </c>
+      <c r="F44" s="6">
+        <v>913</v>
+      </c>
+      <c r="G44" s="6">
+        <v>427</v>
+      </c>
+      <c r="H44" s="5">
+        <f t="shared" ref="H44:H49" si="6">(F44+G44)/(F44-G44)</f>
+        <v>2.7572016460905351</v>
+      </c>
+      <c r="I44" s="3">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>25</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="3">
+        <v>0.754</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="E45" s="5">
+        <f t="shared" si="5"/>
+        <v>1.8614800759013281</v>
+      </c>
+      <c r="F45" s="6">
+        <v>959</v>
+      </c>
+      <c r="G45" s="6">
+        <v>291</v>
+      </c>
+      <c r="H45" s="5">
+        <f t="shared" si="6"/>
+        <v>1.8712574850299402</v>
+      </c>
+      <c r="I45" s="3">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>50</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="3">
+        <v>0.83</v>
+      </c>
+      <c r="D46" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="E46" s="5">
+        <f t="shared" si="5"/>
+        <v>1.0493827160493827</v>
+      </c>
+      <c r="F46" s="6">
+        <v>1067</v>
+      </c>
+      <c r="G46" s="6">
+        <v>16</v>
+      </c>
+      <c r="H46" s="5">
+        <f t="shared" si="6"/>
+        <v>1.0304471931493815</v>
+      </c>
+      <c r="I46" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="11">
+        <v>100</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="11">
+        <v>0.95</v>
+      </c>
+      <c r="D47" s="11">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="E47" s="13">
+        <f t="shared" si="5"/>
+        <v>1.8023598820058999</v>
+      </c>
+      <c r="F47" s="14">
+        <v>1205</v>
+      </c>
+      <c r="G47" s="14">
+        <v>333</v>
+      </c>
+      <c r="H47" s="13">
+        <f t="shared" si="6"/>
+        <v>1.7637614678899083</v>
+      </c>
+      <c r="I47" s="11">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="11">
+        <v>150</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="11">
+        <v>1.0329999999999999</v>
+      </c>
+      <c r="D48" s="11">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="E48" s="13">
+        <f t="shared" si="5"/>
+        <v>2.6958855098389982</v>
+      </c>
+      <c r="F48" s="14">
+        <v>1310</v>
+      </c>
+      <c r="G48" s="14">
+        <v>595</v>
+      </c>
+      <c r="H48" s="13">
+        <f t="shared" si="6"/>
+        <v>2.6643356643356642</v>
+      </c>
+      <c r="I48" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="11">
+        <v>200</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="11">
+        <v>1.071</v>
+      </c>
+      <c r="D49" s="11">
+        <v>0.6</v>
+      </c>
+      <c r="E49" s="13">
+        <f t="shared" si="5"/>
+        <v>3.5477707006369426</v>
+      </c>
+      <c r="F49" s="14">
+        <v>1355</v>
+      </c>
+      <c r="G49" s="14">
+        <v>755</v>
+      </c>
+      <c r="H49" s="13">
+        <f t="shared" si="6"/>
+        <v>3.5166666666666666</v>
+      </c>
+      <c r="I49" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B50" s="22"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="24"/>
+      <c r="H50" s="23"/>
+      <c r="I50" s="21"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" s="25"/>
+      <c r="E57" s="25"/>
+      <c r="F57" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G57" s="25"/>
+      <c r="H57" s="25"/>
+    </row>
+    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="3">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="D59" s="3">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="E59" s="5">
+        <f>(C59+D59)/(C59-D59)</f>
+        <v>3.6363636363636376</v>
+      </c>
+      <c r="F59" s="6">
+        <v>908</v>
+      </c>
+      <c r="G59" s="6">
+        <v>521</v>
+      </c>
+      <c r="H59" s="5">
+        <f>(F59+G59)/(F59-G59)</f>
+        <v>3.6925064599483206</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>16.7</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="3">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="D60" s="3">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="E60" s="5">
+        <f t="shared" ref="E60:E65" si="7">(C60+D60)/(C60-D60)</f>
+        <v>2.7551020408163267</v>
+      </c>
+      <c r="F60" s="6">
+        <v>976</v>
+      </c>
+      <c r="G60" s="6">
+        <v>440</v>
+      </c>
+      <c r="H60" s="5">
+        <f t="shared" ref="H60:H65" si="8">(F60+G60)/(F60-G60)</f>
+        <v>2.6417910447761193</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>25</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" s="3">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="D61" s="3">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="E61" s="5">
+        <f t="shared" si="7"/>
+        <v>1.8703703703703702</v>
+      </c>
+      <c r="F61" s="6">
+        <v>987</v>
+      </c>
+      <c r="G61" s="6">
+        <v>302</v>
+      </c>
+      <c r="H61" s="5">
+        <f t="shared" si="8"/>
+        <v>1.8817518248175182</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <v>50</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" s="3">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="D62" s="3">
+        <v>0</v>
+      </c>
+      <c r="E62" s="5">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="F62" s="6">
+        <v>1087</v>
+      </c>
+      <c r="G62" s="6">
+        <v>8</v>
+      </c>
+      <c r="H62" s="5">
+        <f t="shared" si="8"/>
+        <v>1.0148285449490269</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="11">
+        <v>100</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="11">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="D63" s="11">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="E63" s="13">
+        <f t="shared" si="7"/>
+        <v>1.841010401188707</v>
+      </c>
+      <c r="F63" s="14">
+        <v>1214</v>
+      </c>
+      <c r="G63" s="14">
+        <v>364</v>
+      </c>
+      <c r="H63" s="13">
+        <f t="shared" si="8"/>
+        <v>1.8564705882352941</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="11">
+        <v>150</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" s="11">
+        <v>1.01</v>
+      </c>
+      <c r="D64" s="11">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="E64" s="13">
+        <f t="shared" si="7"/>
+        <v>2.8185255198487713</v>
+      </c>
+      <c r="F64" s="14">
+        <v>1286</v>
+      </c>
+      <c r="G64" s="14">
+        <v>610</v>
+      </c>
+      <c r="H64" s="13">
+        <f t="shared" si="8"/>
+        <v>2.804733727810651</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="11">
+        <v>200</v>
+      </c>
+      <c r="B65" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" s="11">
+        <v>1.0449999999999999</v>
+      </c>
+      <c r="D65" s="11">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="E65" s="13">
+        <f t="shared" si="7"/>
+        <v>3.7178329571106095</v>
+      </c>
+      <c r="F65" s="14">
+        <v>1326</v>
+      </c>
+      <c r="G65" s="14">
+        <v>760</v>
+      </c>
+      <c r="H65" s="13">
+        <f t="shared" si="8"/>
+        <v>3.6855123674911661</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C70" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" s="25"/>
+      <c r="E70" s="25"/>
+      <c r="F70" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G70" s="25"/>
+      <c r="H70" s="25"/>
+    </row>
+    <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" s="3">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="D72" s="3">
+        <v>0.995</v>
+      </c>
+      <c r="E72" s="5">
+        <f>(C72+D72)/(C72-D72)</f>
+        <v>-6.5665399239543722</v>
+      </c>
+      <c r="F72" s="6">
+        <v>1120</v>
+      </c>
+      <c r="G72" s="6">
+        <v>777</v>
+      </c>
+      <c r="H72" s="5">
+        <f>(F72+G72)/(F72-G72)</f>
+        <v>5.5306122448979593</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="3">
+        <v>16.7</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" s="3">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="D73" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="E73" s="5">
+        <f t="shared" ref="E73:E78" si="9">(C73+D73)/(C73-D73)</f>
+        <v>-3.0875912408759123</v>
+      </c>
+      <c r="F73" s="6">
+        <v>1124</v>
+      </c>
+      <c r="G73" s="6">
+        <v>680</v>
+      </c>
+      <c r="H73" s="5">
+        <f t="shared" ref="H73:H78" si="10">(F73+G73)/(F73-G73)</f>
+        <v>4.0630630630630629</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="3">
+        <v>25</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" s="3">
+        <v>0.751</v>
+      </c>
+      <c r="D74" s="3">
+        <v>1.03</v>
+      </c>
+      <c r="E74" s="5">
+        <f t="shared" si="9"/>
+        <v>-6.3835125448028673</v>
+      </c>
+      <c r="F74" s="6">
+        <v>1142</v>
+      </c>
+      <c r="G74" s="6">
+        <v>525</v>
+      </c>
+      <c r="H74" s="5">
+        <f t="shared" si="10"/>
+        <v>2.7017828200972449</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="3">
+        <v>50</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C75" s="3">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="D75" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E75" s="5">
+        <f t="shared" si="9"/>
+        <v>4.2294617563739365</v>
+      </c>
+      <c r="F75" s="6">
+        <v>1190</v>
+      </c>
+      <c r="G75" s="6">
+        <v>158</v>
+      </c>
+      <c r="H75" s="5">
+        <f t="shared" si="10"/>
+        <v>1.306201550387597</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="11">
+        <v>100</v>
+      </c>
+      <c r="B76" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" s="11">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="D76" s="11">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="E76" s="13">
+        <f t="shared" si="9"/>
+        <v>3.0123966942148761</v>
+      </c>
+      <c r="F76" s="14">
+        <v>1244</v>
+      </c>
+      <c r="G76" s="14">
+        <v>182</v>
+      </c>
+      <c r="H76" s="13">
+        <f t="shared" si="10"/>
+        <v>1.3427495291902072</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="11">
+        <v>150</v>
+      </c>
+      <c r="B77" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" s="11">
+        <v>1.008</v>
+      </c>
+      <c r="D77" s="11">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="E77" s="13">
+        <f t="shared" si="9"/>
+        <v>2.63898916967509</v>
+      </c>
+      <c r="F77" s="14">
+        <v>1293</v>
+      </c>
+      <c r="G77" s="14">
+        <v>421</v>
+      </c>
+      <c r="H77" s="13">
+        <f t="shared" si="10"/>
+        <v>1.9655963302752293</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="11">
+        <v>200</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" s="11">
+        <v>1.024</v>
+      </c>
+      <c r="D78" s="11">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="E78" s="13">
+        <f t="shared" si="9"/>
+        <v>3.7850467289719623</v>
+      </c>
+      <c r="F78" s="14">
+        <v>1318</v>
+      </c>
+      <c r="G78" s="14">
+        <v>565</v>
+      </c>
+      <c r="H78" s="13">
+        <f t="shared" si="10"/>
+        <v>2.50066401062417</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>24</v>
+      </c>
+      <c r="C88" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D88" s="25"/>
+      <c r="E88" s="25"/>
+      <c r="F88" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G88" s="25"/>
+      <c r="H88" s="25"/>
+    </row>
+    <row r="89" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C90" s="3">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="D90" s="3">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="E90" s="5">
+        <f>(C90+D90)/(C90-D90)</f>
+        <v>3.7379310344827585</v>
+      </c>
+      <c r="F90" s="6">
+        <v>873</v>
+      </c>
+      <c r="G90" s="6">
+        <v>505</v>
+      </c>
+      <c r="H90" s="5">
+        <f>(F90+G90)/(F90-G90)</f>
+        <v>3.7445652173913042</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="3">
+        <v>16.7</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C91" s="3">
+        <v>0.71</v>
+      </c>
+      <c r="D91" s="3">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="E91" s="5">
+        <f t="shared" ref="E91:E96" si="11">(C91+D91)/(C91-D91)</f>
+        <v>2.8482384823848244</v>
+      </c>
+      <c r="F91" s="6">
+        <v>903</v>
+      </c>
+      <c r="G91" s="6">
+        <v>435</v>
+      </c>
+      <c r="H91" s="5">
+        <f t="shared" ref="H91:H96" si="12">(F91+G91)/(F91-G91)</f>
+        <v>2.858974358974359</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="3">
+        <v>25</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C92" s="3">
+        <v>0.752</v>
+      </c>
+      <c r="D92" s="3">
+        <v>0.24</v>
+      </c>
+      <c r="E92" s="5">
+        <f t="shared" si="11"/>
+        <v>1.9375</v>
+      </c>
+      <c r="F92" s="6">
+        <v>953</v>
+      </c>
+      <c r="G92" s="6">
+        <v>310</v>
+      </c>
+      <c r="H92" s="5">
+        <f t="shared" si="12"/>
+        <v>1.9642301710730949</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="3">
+        <v>50</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C93" s="3">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="D93" s="3">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E93" s="5">
+        <f t="shared" si="11"/>
+        <v>1.0288115246098439</v>
+      </c>
+      <c r="F93" s="6">
+        <v>1076</v>
+      </c>
+      <c r="G93" s="6">
+        <v>32</v>
+      </c>
+      <c r="H93" s="5">
+        <f t="shared" si="12"/>
+        <v>1.0613026819923372</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="11">
+        <v>100</v>
+      </c>
+      <c r="B94" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C94" s="11">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="D94" s="11">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="E94" s="13">
+        <f t="shared" si="11"/>
+        <v>1.820289855072464</v>
+      </c>
+      <c r="F94" s="14">
+        <v>1220</v>
+      </c>
+      <c r="G94" s="14">
+        <v>355</v>
+      </c>
+      <c r="H94" s="13">
+        <f t="shared" si="12"/>
+        <v>1.8208092485549132</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="11">
+        <v>150</v>
+      </c>
+      <c r="B95" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C95" s="11">
+        <v>1.054</v>
+      </c>
+      <c r="D95" s="11">
+        <v>0.499</v>
+      </c>
+      <c r="E95" s="13">
+        <f t="shared" si="11"/>
+        <v>2.798198198198198</v>
+      </c>
+      <c r="F95" s="14">
+        <v>1337</v>
+      </c>
+      <c r="G95" s="14">
+        <v>625</v>
+      </c>
+      <c r="H95" s="13">
+        <f t="shared" si="12"/>
+        <v>2.75561797752809</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="11">
+        <v>200</v>
+      </c>
+      <c r="B96" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C96" s="11">
+        <v>1.0960000000000001</v>
+      </c>
+      <c r="D96" s="11">
+        <v>0.63</v>
+      </c>
+      <c r="E96" s="13">
+        <f t="shared" si="11"/>
+        <v>3.7038626609442051</v>
+      </c>
+      <c r="F96" s="14">
+        <v>1390</v>
+      </c>
+      <c r="G96" s="14">
+        <v>795</v>
+      </c>
+      <c r="H96" s="13">
+        <f t="shared" si="12"/>
+        <v>3.672268907563025</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>27</v>
+      </c>
+      <c r="C101" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D101" s="25"/>
+      <c r="E101" s="25"/>
+      <c r="F101" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G101" s="25"/>
+      <c r="H101" s="25"/>
+    </row>
+    <row r="102" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C103" s="3">
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D103" s="3">
+        <v>1.645</v>
+      </c>
+      <c r="E103" s="5">
+        <f>(C103+D103)/(C103-D103)</f>
+        <v>-4.1406249999999991</v>
+      </c>
+      <c r="F103" s="6">
+        <v>535</v>
+      </c>
+      <c r="G103" s="6">
+        <v>990</v>
+      </c>
+      <c r="H103" s="5">
+        <f>(F103+G103)/(F103-G103)</f>
+        <v>-3.3516483516483517</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="3">
+        <v>16.7</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104" s="3">
+        <v>1.0860000000000001</v>
+      </c>
+      <c r="D104" s="3">
+        <v>1.6319999999999999</v>
+      </c>
+      <c r="E104" s="5">
+        <f t="shared" ref="E104:E109" si="13">(C104+D104)/(C104-D104)</f>
+        <v>-4.9780219780219799</v>
+      </c>
+      <c r="F104" s="6">
+        <v>509</v>
+      </c>
+      <c r="G104" s="6">
+        <v>975</v>
+      </c>
+      <c r="H104" s="5">
+        <f t="shared" ref="H104:H109" si="14">(F104+G104)/(F104-G104)</f>
+        <v>-3.1845493562231759</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" s="3">
+        <v>25</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C105" s="3">
+        <v>1.29</v>
+      </c>
+      <c r="D105" s="3">
+        <v>1.6080000000000001</v>
+      </c>
+      <c r="E105" s="5">
+        <f t="shared" si="13"/>
+        <v>-9.1132075471698109</v>
+      </c>
+      <c r="F105" s="6">
+        <v>465</v>
+      </c>
+      <c r="G105" s="6">
+        <v>890</v>
+      </c>
+      <c r="H105" s="5">
+        <f t="shared" si="14"/>
+        <v>-3.1882352941176473</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" s="3">
+        <v>50</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C106" s="3">
+        <v>1.4370000000000001</v>
+      </c>
+      <c r="D106" s="3">
+        <v>1.64</v>
+      </c>
+      <c r="E106" s="5">
+        <f t="shared" si="13"/>
+        <v>-15.157635467980306</v>
+      </c>
+      <c r="F106" s="6">
+        <v>440</v>
+      </c>
+      <c r="G106" s="6">
+        <v>804</v>
+      </c>
+      <c r="H106" s="5">
+        <f t="shared" si="14"/>
+        <v>-3.4175824175824174</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="11">
+        <v>100</v>
+      </c>
+      <c r="B107" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C107" s="11">
+        <v>1.37</v>
+      </c>
+      <c r="D107" s="11">
+        <v>1.63</v>
+      </c>
+      <c r="E107" s="13">
+        <f t="shared" si="13"/>
+        <v>-11.538461538461547</v>
+      </c>
+      <c r="F107" s="14">
+        <v>515</v>
+      </c>
+      <c r="G107" s="14">
+        <v>1225</v>
+      </c>
+      <c r="H107" s="13">
+        <f t="shared" si="14"/>
+        <v>-2.4507042253521125</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="11">
+        <v>150</v>
+      </c>
+      <c r="B108" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C108" s="11">
+        <v>1.35</v>
+      </c>
+      <c r="D108" s="11">
+        <v>1.597</v>
+      </c>
+      <c r="E108" s="13">
+        <f t="shared" si="13"/>
+        <v>-11.931174089068831</v>
+      </c>
+      <c r="F108" s="14">
+        <v>517</v>
+      </c>
+      <c r="G108" s="14">
+        <v>1298</v>
+      </c>
+      <c r="H108" s="13">
+        <f t="shared" si="14"/>
+        <v>-2.323943661971831</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" s="11">
+        <v>200</v>
+      </c>
+      <c r="B109" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C109" s="11">
+        <v>1.3879999999999999</v>
+      </c>
+      <c r="D109" s="11">
+        <v>1.625</v>
+      </c>
+      <c r="E109" s="13">
+        <f t="shared" si="13"/>
+        <v>-12.713080168776365</v>
+      </c>
+      <c r="F109" s="14">
+        <v>1318</v>
+      </c>
+      <c r="G109" s="14">
+        <v>520</v>
+      </c>
+      <c r="H109" s="13">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="17">
+    <mergeCell ref="C101:E101"/>
+    <mergeCell ref="F101:H101"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="C88:E88"/>
+    <mergeCell ref="F88:H88"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="I41:I42"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="F15:H15"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="F28:H28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
post VSWR bridge tests
VSWR measurements at 50MHz still affected
</commit_message>
<xml_diff>
--- a/measurements/24032020 vswr bridge.xlsx
+++ b/measurements/24032020 vswr bridge.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="VSWR Bridge" sheetId="1" r:id="rId1"/>
+    <sheet name="Tuning Solutions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="67">
   <si>
     <t>Aries VSWR tests</t>
   </si>
@@ -135,6 +136,96 @@
   </si>
   <si>
     <t>These measurements suggest the bridge is inoperable at 28MHz. Vr &gt;&gt; Vf.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is aftter Kjell's change of grounding at the RF bridge. </t>
+  </si>
+  <si>
+    <t>typical noise on Fwd ADC measurement +/- 10 samples (low Z) +/- 20 sample (high Z)</t>
+  </si>
+  <si>
+    <t>typical noise on Rev ADC measurement +/- 10 samples (low Z) +/- 40 samples (high Z)</t>
+  </si>
+  <si>
+    <t>The multimeter readings are useless. They record 1.6V Vr but the oscilloscope says no voltage.</t>
+  </si>
+  <si>
+    <t>typical noise on Fwd ADC measurement +/- 10 samples; on Rev ADC +/-40 samples</t>
+  </si>
+  <si>
+    <t>The true VSWR probably ranged 3:1 to 3:1</t>
+  </si>
+  <si>
+    <t>These readings aren't perfect but the best yet! (not sure we would find a VSWR minimum properly)</t>
+  </si>
+  <si>
+    <t>27/3/2020: VSWR bridge connected to ATU. VSWR bridge grounded to DGND; L13 in place</t>
+  </si>
+  <si>
+    <t>28/3/2020: VSWR bridge connected to ATU. L9 20T winding grounded to RF ground; remainder to DGND</t>
+  </si>
+  <si>
+    <t>typical noise on both ADC measurement +/- 5 samples</t>
+  </si>
+  <si>
+    <t>These are the best measurements yet.</t>
+  </si>
+  <si>
+    <t>typical noise on Fwd ADC measurement +/- 8 samples; on Rev ADC +/-7 samples</t>
+  </si>
+  <si>
+    <t>these are good results.</t>
+  </si>
+  <si>
+    <t>High/Low Z sw</t>
+  </si>
+  <si>
+    <t>Antenna analyser</t>
+  </si>
+  <si>
+    <t>algorithm</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>VSWR</t>
+  </si>
+  <si>
+    <t>8:1 Low</t>
+  </si>
+  <si>
+    <t>2:1 High</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>1.9 MHz</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>5:1</t>
+  </si>
+  <si>
+    <t>8:1</t>
+  </si>
+  <si>
+    <t>3.65 MHz</t>
+  </si>
+  <si>
+    <t>50MHz</t>
+  </si>
+  <si>
+    <t>typical noise on Fwd ADC measurement +/- 4 samples; on Rev ADC +/-5 samples</t>
+  </si>
+  <si>
+    <t>these are nor reading well at 50MHz!</t>
   </si>
 </sst>
 </file>
@@ -174,7 +265,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -197,11 +288,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -233,14 +339,30 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -522,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I111"/>
+  <dimension ref="A1:I186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
+      <selection activeCell="A187" sqref="A187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,16 +666,16 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25" t="s">
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -783,16 +905,16 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25" t="s">
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -1022,14 +1144,14 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
@@ -1204,17 +1326,17 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C41" s="25" t="s">
+      <c r="C41" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25" t="s">
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="26" t="s">
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="31" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1243,7 +1365,7 @@
       <c r="H42" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I42" s="26"/>
+      <c r="I42" s="31"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
@@ -1489,16 +1611,16 @@
       <c r="A57" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="25" t="s">
+      <c r="C57" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D57" s="25"/>
-      <c r="E57" s="25"/>
-      <c r="F57" s="25" t="s">
+      <c r="D57" s="29"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G57" s="25"/>
-      <c r="H57" s="25"/>
+      <c r="G57" s="29"/>
+      <c r="H57" s="29"/>
     </row>
     <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
@@ -1736,16 +1858,16 @@
       <c r="A70" t="s">
         <v>27</v>
       </c>
-      <c r="C70" s="25" t="s">
+      <c r="C70" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D70" s="25"/>
-      <c r="E70" s="25"/>
-      <c r="F70" s="25" t="s">
+      <c r="D70" s="29"/>
+      <c r="E70" s="29"/>
+      <c r="F70" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G70" s="25"/>
-      <c r="H70" s="25"/>
+      <c r="G70" s="29"/>
+      <c r="H70" s="29"/>
     </row>
     <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
@@ -1993,16 +2115,16 @@
       <c r="A88" t="s">
         <v>24</v>
       </c>
-      <c r="C88" s="25" t="s">
+      <c r="C88" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D88" s="25"/>
-      <c r="E88" s="25"/>
-      <c r="F88" s="25" t="s">
+      <c r="D88" s="29"/>
+      <c r="E88" s="29"/>
+      <c r="F88" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G88" s="25"/>
-      <c r="H88" s="25"/>
+      <c r="G88" s="29"/>
+      <c r="H88" s="29"/>
     </row>
     <row r="89" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
@@ -2245,16 +2367,16 @@
       <c r="A101" t="s">
         <v>27</v>
       </c>
-      <c r="C101" s="25" t="s">
+      <c r="C101" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D101" s="25"/>
-      <c r="E101" s="25"/>
-      <c r="F101" s="25" t="s">
+      <c r="D101" s="29"/>
+      <c r="E101" s="29"/>
+      <c r="F101" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G101" s="25"/>
-      <c r="H101" s="25"/>
+      <c r="G101" s="29"/>
+      <c r="H101" s="29"/>
     </row>
     <row r="102" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
@@ -2334,7 +2456,7 @@
         <v>975</v>
       </c>
       <c r="H104" s="5">
-        <f t="shared" ref="H104:H109" si="14">(F104+G104)/(F104-G104)</f>
+        <f t="shared" ref="H104:H108" si="14">(F104+G104)/(F104-G104)</f>
         <v>-3.1845493562231759</v>
       </c>
     </row>
@@ -2487,8 +2609,1095 @@
         <v>36</v>
       </c>
     </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>24</v>
+      </c>
+      <c r="C117" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D117" s="29"/>
+      <c r="E117" s="29"/>
+      <c r="F117" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G117" s="29"/>
+      <c r="H117" s="29"/>
+    </row>
+    <row r="118" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G118" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H118" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C119" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="D119" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E119" s="5">
+        <f>(C119+D119)/(C119-D119)</f>
+        <v>3.6666666666666679</v>
+      </c>
+      <c r="F119" s="6">
+        <v>894</v>
+      </c>
+      <c r="G119" s="6">
+        <v>510</v>
+      </c>
+      <c r="H119" s="5">
+        <f>(F119+G119)/(F119-G119)</f>
+        <v>3.65625</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" s="3">
+        <v>16.7</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C120" s="3">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="D120" s="3">
+        <v>0.34</v>
+      </c>
+      <c r="E120" s="5">
+        <f t="shared" ref="E120:E125" si="15">(C120+D120)/(C120-D120)</f>
+        <v>2.7801047120418851</v>
+      </c>
+      <c r="F120" s="6">
+        <v>920</v>
+      </c>
+      <c r="G120" s="6">
+        <v>435</v>
+      </c>
+      <c r="H120" s="5">
+        <f t="shared" ref="H120:H125" si="16">(F120+G120)/(F120-G120)</f>
+        <v>2.7938144329896906</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" s="3">
+        <v>25</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C121" s="3">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="D121" s="3">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="E121" s="5">
+        <f t="shared" si="15"/>
+        <v>1.8754716981132074</v>
+      </c>
+      <c r="F121" s="6">
+        <v>970</v>
+      </c>
+      <c r="G121" s="6">
+        <v>305</v>
+      </c>
+      <c r="H121" s="5">
+        <f t="shared" si="16"/>
+        <v>1.9172932330827068</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" s="3">
+        <v>50</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C122" s="3">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="D122" s="3">
+        <v>0</v>
+      </c>
+      <c r="E122" s="5">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="F122" s="6">
+        <v>1085</v>
+      </c>
+      <c r="G122" s="6">
+        <v>15</v>
+      </c>
+      <c r="H122" s="5">
+        <f t="shared" si="16"/>
+        <v>1.02803738317757</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" s="11">
+        <v>100</v>
+      </c>
+      <c r="B123" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C123" s="11">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="D123" s="11">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="E123" s="13">
+        <f t="shared" si="15"/>
+        <v>1.8318840579710147</v>
+      </c>
+      <c r="F123" s="14">
+        <v>1240</v>
+      </c>
+      <c r="G123" s="14">
+        <v>354</v>
+      </c>
+      <c r="H123" s="13">
+        <f t="shared" si="16"/>
+        <v>1.7990970654627541</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="11">
+        <v>150</v>
+      </c>
+      <c r="B124" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C124" s="11">
+        <v>1.048</v>
+      </c>
+      <c r="D124" s="11">
+        <v>0.496</v>
+      </c>
+      <c r="E124" s="13">
+        <f t="shared" si="15"/>
+        <v>2.7971014492753623</v>
+      </c>
+      <c r="F124" s="14">
+        <v>1333</v>
+      </c>
+      <c r="G124" s="14">
+        <v>627</v>
+      </c>
+      <c r="H124" s="13">
+        <f t="shared" si="16"/>
+        <v>2.7762039660056659</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" s="11">
+        <v>200</v>
+      </c>
+      <c r="B125" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C125" s="11">
+        <v>1.0920000000000001</v>
+      </c>
+      <c r="D125" s="11">
+        <v>0.626</v>
+      </c>
+      <c r="E125" s="13">
+        <f t="shared" si="15"/>
+        <v>3.6866952789699563</v>
+      </c>
+      <c r="F125" s="14">
+        <v>1390</v>
+      </c>
+      <c r="G125" s="14">
+        <v>792</v>
+      </c>
+      <c r="H125" s="13">
+        <f t="shared" si="16"/>
+        <v>3.6488294314381271</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>27</v>
+      </c>
+      <c r="C130" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D130" s="29"/>
+      <c r="E130" s="29"/>
+      <c r="F130" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G130" s="29"/>
+      <c r="H130" s="29"/>
+    </row>
+    <row r="131" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G131" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H131" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C132" s="3"/>
+      <c r="D132" s="3"/>
+      <c r="E132" s="5"/>
+      <c r="F132" s="6">
+        <v>920</v>
+      </c>
+      <c r="G132" s="6">
+        <v>315</v>
+      </c>
+      <c r="H132" s="5">
+        <f>(F132+G132)/(F132-G132)</f>
+        <v>2.0413223140495869</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" s="3">
+        <v>16.7</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C133" s="3"/>
+      <c r="D133" s="3"/>
+      <c r="E133" s="5"/>
+      <c r="F133" s="6">
+        <v>962</v>
+      </c>
+      <c r="G133" s="6">
+        <v>197</v>
+      </c>
+      <c r="H133" s="5">
+        <f t="shared" ref="H133:H138" si="17">(F133+G133)/(F133-G133)</f>
+        <v>1.515032679738562</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134" s="3">
+        <v>25</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C134" s="3"/>
+      <c r="D134" s="3"/>
+      <c r="E134" s="5"/>
+      <c r="F134" s="6">
+        <v>963</v>
+      </c>
+      <c r="G134" s="6">
+        <v>190</v>
+      </c>
+      <c r="H134" s="5">
+        <f t="shared" si="17"/>
+        <v>1.4915912031047867</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A135" s="3">
+        <v>50</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C135" s="3"/>
+      <c r="D135" s="3"/>
+      <c r="E135" s="5"/>
+      <c r="F135" s="6">
+        <v>1090</v>
+      </c>
+      <c r="G135" s="6">
+        <v>60</v>
+      </c>
+      <c r="H135" s="5">
+        <f t="shared" si="17"/>
+        <v>1.116504854368932</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" s="11">
+        <v>100</v>
+      </c>
+      <c r="B136" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C136" s="11"/>
+      <c r="D136" s="11"/>
+      <c r="E136" s="13"/>
+      <c r="F136" s="14">
+        <v>1188</v>
+      </c>
+      <c r="G136" s="14">
+        <v>289</v>
+      </c>
+      <c r="H136" s="13">
+        <f t="shared" si="17"/>
+        <v>1.64293659621802</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" s="11">
+        <v>150</v>
+      </c>
+      <c r="B137" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C137" s="11"/>
+      <c r="D137" s="11"/>
+      <c r="E137" s="13"/>
+      <c r="F137" s="14">
+        <v>1243</v>
+      </c>
+      <c r="G137" s="14">
+        <v>455</v>
+      </c>
+      <c r="H137" s="13">
+        <f t="shared" si="17"/>
+        <v>2.1548223350253806</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="11">
+        <v>200</v>
+      </c>
+      <c r="B138" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C138" s="11"/>
+      <c r="D138" s="11"/>
+      <c r="E138" s="13"/>
+      <c r="F138" s="14">
+        <v>1260</v>
+      </c>
+      <c r="G138" s="14">
+        <v>540</v>
+      </c>
+      <c r="H138" s="13">
+        <f t="shared" si="17"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>24</v>
+      </c>
+      <c r="C149" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D149" s="29"/>
+      <c r="E149" s="29"/>
+      <c r="F149" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G149" s="29"/>
+      <c r="H149" s="29"/>
+    </row>
+    <row r="150" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G150" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H150" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A151" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="B151" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C151" s="3"/>
+      <c r="D151" s="3"/>
+      <c r="E151" s="5"/>
+      <c r="F151" s="6">
+        <v>875</v>
+      </c>
+      <c r="G151" s="6">
+        <v>498</v>
+      </c>
+      <c r="H151" s="5">
+        <f>(F151+G151)/(F151-G151)</f>
+        <v>3.6419098143236073</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A152" s="3">
+        <v>16.7</v>
+      </c>
+      <c r="B152" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C152" s="3"/>
+      <c r="D152" s="3"/>
+      <c r="E152" s="5"/>
+      <c r="F152" s="6">
+        <v>899</v>
+      </c>
+      <c r="G152" s="6">
+        <v>420</v>
+      </c>
+      <c r="H152" s="5">
+        <f t="shared" ref="H152:H157" si="18">(F152+G152)/(F152-G152)</f>
+        <v>2.7536534446764094</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A153" s="3">
+        <v>25</v>
+      </c>
+      <c r="B153" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C153" s="3"/>
+      <c r="D153" s="3"/>
+      <c r="E153" s="5"/>
+      <c r="F153" s="6">
+        <v>951</v>
+      </c>
+      <c r="G153" s="6">
+        <v>289</v>
+      </c>
+      <c r="H153" s="5">
+        <f t="shared" si="18"/>
+        <v>1.8731117824773413</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A154" s="3">
+        <v>50</v>
+      </c>
+      <c r="B154" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C154" s="3"/>
+      <c r="D154" s="3"/>
+      <c r="E154" s="5"/>
+      <c r="F154" s="6">
+        <v>1064</v>
+      </c>
+      <c r="G154" s="6">
+        <v>10</v>
+      </c>
+      <c r="H154" s="5">
+        <f t="shared" si="18"/>
+        <v>1.0189753320683113</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A155" s="11">
+        <v>100</v>
+      </c>
+      <c r="B155" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C155" s="11"/>
+      <c r="D155" s="11"/>
+      <c r="E155" s="13"/>
+      <c r="F155" s="14">
+        <v>1210</v>
+      </c>
+      <c r="G155" s="14">
+        <v>364</v>
+      </c>
+      <c r="H155" s="13">
+        <f t="shared" si="18"/>
+        <v>1.8605200945626477</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A156" s="11">
+        <v>150</v>
+      </c>
+      <c r="B156" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C156" s="11"/>
+      <c r="D156" s="11"/>
+      <c r="E156" s="13"/>
+      <c r="F156" s="14">
+        <v>1295</v>
+      </c>
+      <c r="G156" s="14">
+        <v>619</v>
+      </c>
+      <c r="H156" s="13">
+        <f t="shared" si="18"/>
+        <v>2.831360946745562</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A157" s="11">
+        <v>200</v>
+      </c>
+      <c r="B157" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C157" s="11"/>
+      <c r="D157" s="11"/>
+      <c r="E157" s="13"/>
+      <c r="F157" s="14">
+        <v>1352</v>
+      </c>
+      <c r="G157" s="14">
+        <v>773</v>
+      </c>
+      <c r="H157" s="13">
+        <f t="shared" si="18"/>
+        <v>3.6701208981001727</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>27</v>
+      </c>
+      <c r="C162" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D162" s="29"/>
+      <c r="E162" s="29"/>
+      <c r="F162" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G162" s="29"/>
+      <c r="H162" s="29"/>
+    </row>
+    <row r="163" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E163" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F163" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G163" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H163" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A164" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="B164" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C164" s="3"/>
+      <c r="D164" s="3"/>
+      <c r="E164" s="5"/>
+      <c r="F164" s="6">
+        <v>1021</v>
+      </c>
+      <c r="G164" s="6">
+        <v>515</v>
+      </c>
+      <c r="H164" s="5">
+        <f>(F164+G164)/(F164-G164)</f>
+        <v>3.0355731225296441</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A165" s="3">
+        <v>16.7</v>
+      </c>
+      <c r="B165" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C165" s="3"/>
+      <c r="D165" s="3"/>
+      <c r="E165" s="5"/>
+      <c r="F165" s="6">
+        <v>1042</v>
+      </c>
+      <c r="G165" s="6">
+        <v>421</v>
+      </c>
+      <c r="H165" s="5">
+        <f t="shared" ref="H165:H170" si="19">(F165+G165)/(F165-G165)</f>
+        <v>2.3558776167471818</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A166" s="3">
+        <v>25</v>
+      </c>
+      <c r="B166" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C166" s="3"/>
+      <c r="D166" s="3"/>
+      <c r="E166" s="5"/>
+      <c r="F166" s="6">
+        <v>1066</v>
+      </c>
+      <c r="G166" s="6">
+        <v>289</v>
+      </c>
+      <c r="H166" s="5">
+        <f t="shared" si="19"/>
+        <v>1.7438867438867438</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A167" s="3">
+        <v>50</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C167" s="3"/>
+      <c r="D167" s="3"/>
+      <c r="E167" s="5"/>
+      <c r="F167" s="6">
+        <v>1129</v>
+      </c>
+      <c r="G167" s="6">
+        <v>197</v>
+      </c>
+      <c r="H167" s="5">
+        <f t="shared" si="19"/>
+        <v>1.4227467811158798</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A168" s="11">
+        <v>100</v>
+      </c>
+      <c r="B168" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C168" s="11"/>
+      <c r="D168" s="11"/>
+      <c r="E168" s="13"/>
+      <c r="F168" s="14">
+        <v>1193</v>
+      </c>
+      <c r="G168" s="14">
+        <v>476</v>
+      </c>
+      <c r="H168" s="13">
+        <f t="shared" si="19"/>
+        <v>2.3277545327754532</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A169" s="11">
+        <v>150</v>
+      </c>
+      <c r="B169" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C169" s="11"/>
+      <c r="D169" s="11"/>
+      <c r="E169" s="13"/>
+      <c r="F169" s="14">
+        <v>1221</v>
+      </c>
+      <c r="G169" s="14">
+        <v>635</v>
+      </c>
+      <c r="H169" s="13">
+        <f t="shared" si="19"/>
+        <v>3.1672354948805461</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A170" s="11">
+        <v>200</v>
+      </c>
+      <c r="B170" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C170" s="11"/>
+      <c r="D170" s="11"/>
+      <c r="E170" s="13"/>
+      <c r="F170" s="14">
+        <v>1240</v>
+      </c>
+      <c r="G170" s="14">
+        <v>734</v>
+      </c>
+      <c r="H170" s="13">
+        <f t="shared" si="19"/>
+        <v>3.9011857707509883</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>64</v>
+      </c>
+      <c r="C176" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D176" s="29"/>
+      <c r="E176" s="29"/>
+      <c r="F176" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G176" s="29"/>
+      <c r="H176" s="29"/>
+    </row>
+    <row r="177" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A177" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D177" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E177" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F177" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G177" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H177" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A178" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="B178" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C178" s="3"/>
+      <c r="D178" s="3"/>
+      <c r="E178" s="5"/>
+      <c r="F178" s="6">
+        <v>690</v>
+      </c>
+      <c r="G178" s="6">
+        <v>477</v>
+      </c>
+      <c r="H178" s="5">
+        <f>(F178+G178)/(F178-G178)</f>
+        <v>5.47887323943662</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A179" s="3">
+        <v>16.7</v>
+      </c>
+      <c r="B179" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C179" s="3"/>
+      <c r="D179" s="3"/>
+      <c r="E179" s="5"/>
+      <c r="F179" s="6">
+        <v>690</v>
+      </c>
+      <c r="G179" s="6">
+        <v>460</v>
+      </c>
+      <c r="H179" s="5">
+        <f t="shared" ref="H179:H184" si="20">(F179+G179)/(F179-G179)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A180" s="3">
+        <v>25</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C180" s="3"/>
+      <c r="D180" s="3"/>
+      <c r="E180" s="5"/>
+      <c r="F180" s="6">
+        <v>695</v>
+      </c>
+      <c r="G180" s="6">
+        <v>425</v>
+      </c>
+      <c r="H180" s="5">
+        <f t="shared" si="20"/>
+        <v>4.1481481481481479</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A181" s="3">
+        <v>50</v>
+      </c>
+      <c r="B181" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C181" s="3"/>
+      <c r="D181" s="3"/>
+      <c r="E181" s="5"/>
+      <c r="F181" s="6">
+        <v>718</v>
+      </c>
+      <c r="G181" s="6">
+        <v>307</v>
+      </c>
+      <c r="H181" s="5">
+        <f t="shared" si="20"/>
+        <v>2.4939172749391729</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A182" s="11">
+        <v>100</v>
+      </c>
+      <c r="B182" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C182" s="11"/>
+      <c r="D182" s="11"/>
+      <c r="E182" s="13"/>
+      <c r="F182" s="14">
+        <v>695</v>
+      </c>
+      <c r="G182" s="14">
+        <v>412</v>
+      </c>
+      <c r="H182" s="13">
+        <f t="shared" si="20"/>
+        <v>3.9116607773851588</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A183" s="11">
+        <v>150</v>
+      </c>
+      <c r="B183" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C183" s="11"/>
+      <c r="D183" s="11"/>
+      <c r="E183" s="13"/>
+      <c r="F183" s="14">
+        <v>689</v>
+      </c>
+      <c r="G183" s="14">
+        <v>443</v>
+      </c>
+      <c r="H183" s="13">
+        <f t="shared" si="20"/>
+        <v>4.6016260162601625</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A184" s="11">
+        <v>200</v>
+      </c>
+      <c r="B184" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C184" s="11"/>
+      <c r="D184" s="11"/>
+      <c r="E184" s="13"/>
+      <c r="F184" s="14">
+        <v>685</v>
+      </c>
+      <c r="G184" s="14">
+        <v>467</v>
+      </c>
+      <c r="H184" s="13">
+        <f t="shared" si="20"/>
+        <v>5.2844036697247709</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="27">
+    <mergeCell ref="C176:E176"/>
+    <mergeCell ref="F176:H176"/>
+    <mergeCell ref="C149:E149"/>
+    <mergeCell ref="F149:H149"/>
+    <mergeCell ref="C162:E162"/>
+    <mergeCell ref="F162:H162"/>
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="C117:E117"/>
+    <mergeCell ref="F117:H117"/>
+    <mergeCell ref="C130:E130"/>
+    <mergeCell ref="F130:H130"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="F41:H41"/>
     <mergeCell ref="C101:E101"/>
     <mergeCell ref="F101:H101"/>
     <mergeCell ref="C57:E57"/>
@@ -2497,9 +3706,6 @@
     <mergeCell ref="F70:H70"/>
     <mergeCell ref="C88:E88"/>
     <mergeCell ref="F88:H88"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="I41:I42"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="C15:E15"/>
@@ -2510,4 +3716,557 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:8" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="32"/>
+      <c r="C3" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="26">
+        <v>35</v>
+      </c>
+      <c r="D4" s="26">
+        <v>255</v>
+      </c>
+      <c r="E4" s="28">
+        <v>1.4</v>
+      </c>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="26">
+        <v>40</v>
+      </c>
+      <c r="D5" s="26">
+        <v>230</v>
+      </c>
+      <c r="E5" s="28">
+        <v>1.2</v>
+      </c>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="26">
+        <v>40</v>
+      </c>
+      <c r="D6" s="26">
+        <v>224</v>
+      </c>
+      <c r="E6" s="28">
+        <v>1.2</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="26">
+        <v>48</v>
+      </c>
+      <c r="D7" s="26">
+        <v>184</v>
+      </c>
+      <c r="E7" s="28">
+        <v>1.2</v>
+      </c>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="26">
+        <v>0</v>
+      </c>
+      <c r="D8" s="26">
+        <v>48</v>
+      </c>
+      <c r="E8" s="28">
+        <v>1.3</v>
+      </c>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="26">
+        <v>0</v>
+      </c>
+      <c r="D9" s="26">
+        <v>16</v>
+      </c>
+      <c r="E9" s="28">
+        <v>1</v>
+      </c>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="26">
+        <v>76</v>
+      </c>
+      <c r="D10" s="26">
+        <v>55</v>
+      </c>
+      <c r="E10" s="28">
+        <v>1.3</v>
+      </c>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="26">
+        <v>119</v>
+      </c>
+      <c r="D11" s="26">
+        <v>50</v>
+      </c>
+      <c r="E11" s="28">
+        <v>1.3</v>
+      </c>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="26">
+        <v>157</v>
+      </c>
+      <c r="D12" s="26">
+        <v>46</v>
+      </c>
+      <c r="E12" s="28">
+        <v>1.4</v>
+      </c>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="26">
+        <v>179</v>
+      </c>
+      <c r="D13" s="26">
+        <v>43</v>
+      </c>
+      <c r="E13" s="28">
+        <v>1.4</v>
+      </c>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="26">
+        <v>246</v>
+      </c>
+      <c r="D14" s="26">
+        <v>32</v>
+      </c>
+      <c r="E14" s="28">
+        <v>1.4</v>
+      </c>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="32"/>
+      <c r="C19" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="26">
+        <v>2</v>
+      </c>
+      <c r="D20" s="26">
+        <v>171</v>
+      </c>
+      <c r="E20" s="26">
+        <v>1.5</v>
+      </c>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="26">
+        <v>8</v>
+      </c>
+      <c r="D21" s="26">
+        <v>129</v>
+      </c>
+      <c r="E21" s="26">
+        <v>1.3</v>
+      </c>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="26">
+        <v>11</v>
+      </c>
+      <c r="D22" s="26">
+        <v>117</v>
+      </c>
+      <c r="E22" s="26">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="26">
+        <v>14</v>
+      </c>
+      <c r="D23" s="26">
+        <v>96</v>
+      </c>
+      <c r="E23" s="26">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="26">
+        <v>20</v>
+      </c>
+      <c r="D24" s="26">
+        <v>52</v>
+      </c>
+      <c r="E24" s="26">
+        <v>1.3</v>
+      </c>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="26">
+        <v>0</v>
+      </c>
+      <c r="D25" s="26">
+        <v>8</v>
+      </c>
+      <c r="E25" s="26">
+        <v>1</v>
+      </c>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="26">
+        <v>31</v>
+      </c>
+      <c r="D26" s="26">
+        <v>29</v>
+      </c>
+      <c r="E26" s="26">
+        <v>1.3</v>
+      </c>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="26">
+        <v>63</v>
+      </c>
+      <c r="D27" s="26">
+        <v>23</v>
+      </c>
+      <c r="E27" s="26">
+        <v>1.2</v>
+      </c>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="26">
+        <v>77</v>
+      </c>
+      <c r="D28" s="26">
+        <v>19</v>
+      </c>
+      <c r="E28" s="26">
+        <v>1.2</v>
+      </c>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="26">
+        <v>88</v>
+      </c>
+      <c r="D29" s="26">
+        <v>16</v>
+      </c>
+      <c r="E29" s="26">
+        <v>1.2</v>
+      </c>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="26">
+        <v>134</v>
+      </c>
+      <c r="D30" s="26">
+        <v>11</v>
+      </c>
+      <c r="E30" s="26">
+        <v>1.2</v>
+      </c>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:H18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>